<commit_message>
agregando todo lo nuevo de 3ero
</commit_message>
<xml_diff>
--- a/carrera.xlsx
+++ b/carrera.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\importante\Facultad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\importante\Facultad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8420849-1FEA-4730-A364-A88C2D91E776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2F3004-4CE2-4135-BC5C-72F37DA68384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{9EAF091F-EF83-4EF9-8EEF-EE93EA71BDCC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{9EAF091F-EF83-4EF9-8EEF-EE93EA71BDCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -578,6 +578,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -916,7 +917,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,16 +1189,16 @@
       <c r="N15" s="16"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="24">
         <v>2</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="21"/>
+      <c r="D16" s="41"/>
       <c r="E16" s="11"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -1222,18 +1223,18 @@
       <c r="N17" s="16"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="24">
         <v>2</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="1"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="26"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="N18" s="17"/>

</xml_diff>